<commit_message>
separete file for b750
</commit_message>
<xml_diff>
--- a/ConfigletBase/input/Template2c.xlsx
+++ b/ConfigletBase/input/Template2c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://warnermedia-my.sharepoint.com/personal/fred_renner_warnermedia_com/Documents/net-programming/ConfigletBase/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{D229951C-79AB-A842-B3F4-D6D3E2F3E23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9DD643F-02D1-3643-AA20-46E846D4086C}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{D229951C-79AB-A842-B3F4-D6D3E2F3E23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{906EE4EB-E5D1-8840-A1BB-80F7CBCBA6CF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20660" windowHeight="27200" xr2:uid="{10738699-15E7-BB48-982D-CDB51ACC3477}"/>
+    <workbookView xWindow="20640" yWindow="1300" windowWidth="24800" windowHeight="23640" xr2:uid="{10738699-15E7-BB48-982D-CDB51ACC3477}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Building</t>
   </si>
@@ -74,27 +74,15 @@
     <t>SPEC_VLAN</t>
   </si>
   <si>
-    <t>corportate_passthru</t>
-  </si>
-  <si>
     <t>Managemet Mask</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
-    <t>1.1.1.24</t>
-  </si>
-  <si>
     <t>Uplink Addr 1</t>
   </si>
   <si>
     <t>Uplink Addr 2</t>
   </si>
   <si>
-    <t>2.2.2.2</t>
-  </si>
-  <si>
     <t>LoopbackID</t>
   </si>
   <si>
@@ -134,18 +122,6 @@
     <t>SNMPLOC</t>
   </si>
   <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>165.178.15.1</t>
-  </si>
-  <si>
-    <t>10.152.15.1</t>
-  </si>
-  <si>
-    <t>10.152.18.1</t>
-  </si>
-  <si>
     <t>SP_VLAN_a</t>
   </si>
   <si>
@@ -158,13 +134,31 @@
     <t>Spine Interface2</t>
   </si>
   <si>
-    <t>E1/1/1</t>
-  </si>
-  <si>
-    <t>E2/1/1</t>
-  </si>
-  <si>
-    <t>B750 1st Fl Rack Room # 1XXX</t>
+    <t>Lo2</t>
+  </si>
+  <si>
+    <t>10.129.75.1</t>
+  </si>
+  <si>
+    <t>10.129.250.1</t>
+  </si>
+  <si>
+    <t>10.129.252.1</t>
+  </si>
+  <si>
+    <t>10.129.244.1</t>
+  </si>
+  <si>
+    <t>E3/12</t>
+  </si>
+  <si>
+    <t>10.129.2.75</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>B750 2CT2 1st Floor FanLab Rack Room</t>
   </si>
 </sst>
 </file>
@@ -283,9 +277,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -313,6 +307,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,7 +613,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,7 +622,7 @@
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,7 +630,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -640,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -648,11 +646,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -660,59 +658,56 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -720,7 +715,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -728,11 +723,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -773,31 +768,31 @@
         <v>7</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>65012.15</v>
+        <v>65012.104200000002</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1">
         <v>24</v>
@@ -805,15 +800,15 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1">
         <v>23</v>
@@ -821,15 +816,15 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1">
         <v>23</v>
@@ -837,15 +832,15 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>23</v>
@@ -869,24 +864,24 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B35" s="5">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B36" s="1">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -895,10 +890,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>